<commit_message>
thorough updates of results
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/results/improvements/local_optimum_1000.xlsx
+++ b/dmsan/bwaise/results/improvements/local_optimum_1000.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/bwaise/results/improvements/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_DBF485B191E6E8BF891C87E6DAAD73CDD1B2D423" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8E1F5B7-EDB1-8B4B-824C-36D0F1A9E273}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -103,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,14 +161,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -221,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,27 +239,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,24 +273,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -498,16 +448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E27"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="B1" s="1">
         <v>1</v>
       </c>
@@ -521,151 +469,151 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>8.3000000000000004E-2</v>
+        <v>0.083</v>
       </c>
       <c r="C2">
-        <v>0.39600000000000002</v>
+        <v>0.396</v>
       </c>
       <c r="D2">
-        <v>0.61199999999999999</v>
+        <v>0.612</v>
       </c>
       <c r="E2">
-        <v>0.86899999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.869</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C3">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D3">
-        <v>0.60899999999999999</v>
+        <v>0.609</v>
       </c>
       <c r="E3">
-        <v>0.86399999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.864</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C4">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D4">
         <v>0.61</v>
       </c>
       <c r="E4">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.866</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C5">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D5">
         <v>0.61</v>
       </c>
       <c r="E5">
-        <v>0.86799999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C6">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D6">
         <v>0.61</v>
       </c>
       <c r="E6">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.866</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>8.4000000000000005E-2</v>
+        <v>0.08400000000000001</v>
       </c>
       <c r="C7">
-        <v>0.39600000000000002</v>
+        <v>0.396</v>
       </c>
       <c r="D7">
-        <v>0.61199999999999999</v>
+        <v>0.612</v>
       </c>
       <c r="E7">
-        <v>0.86899999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.869</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C8">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D8">
         <v>0.61</v>
       </c>
       <c r="E8">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.866</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>8.8999999999999996E-2</v>
+        <v>0.089</v>
       </c>
       <c r="C9">
-        <v>0.39800000000000002</v>
+        <v>0.398</v>
       </c>
       <c r="D9">
-        <v>0.61799999999999999</v>
+        <v>0.618</v>
       </c>
       <c r="E9">
         <v>0.872</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>9.4E-2</v>
+        <v>0.094</v>
       </c>
       <c r="C10">
-        <v>0.40300000000000002</v>
+        <v>0.403</v>
       </c>
       <c r="D10">
         <v>0.624</v>
@@ -674,15 +622,15 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.16500000000000001</v>
+        <v>0.165</v>
       </c>
       <c r="C11">
-        <v>0.51100000000000001</v>
+        <v>0.511</v>
       </c>
       <c r="D11">
         <v>0.75</v>
@@ -691,15 +639,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C12">
-        <v>0.39900000000000002</v>
+        <v>0.399</v>
       </c>
       <c r="D12">
         <v>0.621</v>
@@ -708,41 +656,41 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C13">
-        <v>0.39800000000000002</v>
+        <v>0.398</v>
       </c>
       <c r="D13">
-        <v>0.61799999999999999</v>
+        <v>0.618</v>
       </c>
       <c r="E13">
         <v>0.877</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C14">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D14">
         <v>0.61</v>
       </c>
       <c r="E14">
-        <v>0.86699999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.867</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -750,58 +698,58 @@
         <v>0.183</v>
       </c>
       <c r="C15">
-        <v>0.52800000000000002</v>
+        <v>0.528</v>
       </c>
       <c r="D15">
-        <v>0.76100000000000001</v>
+        <v>0.761</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C16">
-        <v>0.39700000000000002</v>
+        <v>0.397</v>
       </c>
       <c r="D16">
-        <v>0.61699999999999999</v>
+        <v>0.617</v>
       </c>
       <c r="E16">
         <v>0.873</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C17">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D17">
         <v>0.61</v>
       </c>
       <c r="E17">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.866</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C18">
-        <v>0.39700000000000002</v>
+        <v>0.397</v>
       </c>
       <c r="D18">
         <v>0.624</v>
@@ -810,7 +758,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -821,125 +769,125 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0.41099999999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.411</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C21">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D21">
         <v>0.61</v>
       </c>
       <c r="E21">
-        <v>0.86699999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.867</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0.14699999999999999</v>
+        <v>0.147</v>
       </c>
       <c r="C22">
-        <v>0.58099999999999996</v>
+        <v>0.581</v>
       </c>
       <c r="D22">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.866</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23">
-        <v>8.2000000000000003E-2</v>
+        <v>0.082</v>
       </c>
       <c r="C23">
-        <v>0.39400000000000002</v>
+        <v>0.394</v>
       </c>
       <c r="D23">
         <v>0.61</v>
       </c>
       <c r="E23">
-        <v>0.86599999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.866</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24">
-        <v>8.3000000000000004E-2</v>
+        <v>0.083</v>
       </c>
       <c r="C24">
-        <v>0.41399999999999998</v>
+        <v>0.414</v>
       </c>
       <c r="D24">
-        <v>0.63800000000000001</v>
+        <v>0.638</v>
       </c>
       <c r="E24">
-        <v>0.88800000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.888</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25">
-        <v>8.5999999999999993E-2</v>
+        <v>0.08599999999999999</v>
       </c>
       <c r="C25">
-        <v>0.44800000000000001</v>
+        <v>0.448</v>
       </c>
       <c r="D25">
-        <v>0.69199999999999995</v>
+        <v>0.6919999999999999</v>
       </c>
       <c r="E25">
-        <v>0.88100000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>0.881</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B26">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="C26">
-        <v>0.35899999999999999</v>
+        <v>0.359</v>
       </c>
       <c r="D26">
-        <v>0.56299999999999994</v>
+        <v>0.5629999999999999</v>
       </c>
       <c r="E26">
         <v>0.87</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B27">
-        <v>8.3000000000000004E-2</v>
+        <v>0.083</v>
       </c>
       <c r="C27">
-        <v>0.42299999999999999</v>
+        <v>0.423</v>
       </c>
       <c r="D27">
-        <v>0.65100000000000002</v>
+        <v>0.651</v>
       </c>
       <c r="E27">
         <v>0.877</v>

</xml_diff>